<commit_message>
no major changes. addedd a flood management test file. Rest should be staying the same.
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/test_results.xlsx
+++ b/heliostrome/jip_project/results/test_results.xlsx
@@ -525,10 +525,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>24.0958</v>
+        <v>24.1</v>
       </c>
       <c r="C2" t="n">
-        <v>90.41249999999999</v>
+        <v>90.41</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>40179</v>
@@ -584,10 +584,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>24.0958</v>
+        <v>24.1</v>
       </c>
       <c r="C3" t="n">
-        <v>90.41249999999999</v>
+        <v>90.41</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>40179</v>
@@ -643,10 +643,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>24.0958</v>
+        <v>24.1</v>
       </c>
       <c r="C4" t="n">
-        <v>90.41249999999999</v>
+        <v>90.41</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>40179</v>
@@ -702,10 +702,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>24.0958</v>
+        <v>24.1</v>
       </c>
       <c r="C5" t="n">
-        <v>90.41249999999999</v>
+        <v>90.41</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>40179</v>
@@ -761,10 +761,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>24.0958</v>
+        <v>24.1</v>
       </c>
       <c r="C6" t="n">
-        <v>90.41249999999999</v>
+        <v>90.41</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>40179</v>
@@ -820,10 +820,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>24.0958</v>
+        <v>24.1</v>
       </c>
       <c r="C7" t="n">
-        <v>90.41249999999999</v>
+        <v>90.41</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>40179</v>
@@ -879,10 +879,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>24.0958</v>
+        <v>24.1</v>
       </c>
       <c r="C8" t="n">
-        <v>90.41249999999999</v>
+        <v>90.41</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>40179</v>
@@ -938,10 +938,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>24.91625</v>
+        <v>24.92</v>
       </c>
       <c r="C9" t="n">
-        <v>89.941109</v>
+        <v>89.94</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>40179</v>
@@ -997,10 +997,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>24.91625</v>
+        <v>24.92</v>
       </c>
       <c r="C10" t="n">
-        <v>89.941109</v>
+        <v>89.94</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>40179</v>
@@ -1056,10 +1056,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>24.91625</v>
+        <v>24.92</v>
       </c>
       <c r="C11" t="n">
-        <v>89.941109</v>
+        <v>89.94</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>40179</v>
@@ -1115,10 +1115,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>24.91625</v>
+        <v>24.92</v>
       </c>
       <c r="C12" t="n">
-        <v>89.941109</v>
+        <v>89.94</v>
       </c>
       <c r="D12" s="2" t="n">
         <v>40179</v>
@@ -1174,10 +1174,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>24.91625</v>
+        <v>24.92</v>
       </c>
       <c r="C13" t="n">
-        <v>89.941109</v>
+        <v>89.94</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>40179</v>
@@ -1215,7 +1215,7 @@
       </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="n">
-        <v>35.175</v>
+        <v>35.18</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
@@ -1235,10 +1235,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>24.91625</v>
+        <v>24.92</v>
       </c>
       <c r="C14" t="n">
-        <v>89.941109</v>
+        <v>89.94</v>
       </c>
       <c r="D14" s="2" t="n">
         <v>40179</v>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
-        <v>32.655</v>
+        <v>32.66</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
@@ -1296,10 +1296,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>24.0958</v>
+        <v>24.1</v>
       </c>
       <c r="C15" t="n">
-        <v>90.41249999999999</v>
+        <v>90.41</v>
       </c>
       <c r="D15" s="2" t="n">
         <v>40179</v>
@@ -1355,10 +1355,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>23.490938</v>
+        <v>23.49</v>
       </c>
       <c r="C16" t="n">
-        <v>89.42113500000001</v>
+        <v>89.42</v>
       </c>
       <c r="D16" s="2" t="n">
         <v>40179</v>
@@ -1414,10 +1414,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>22.7049694444444</v>
+        <v>22.7</v>
       </c>
       <c r="C17" t="n">
-        <v>90.37013055555551</v>
+        <v>90.37</v>
       </c>
       <c r="D17" s="2" t="n">
         <v>40179</v>
@@ -1543,7 +1543,7 @@
         <v>285</v>
       </c>
       <c r="F2" t="n">
-        <v>8.258510109442415</v>
+        <v>8.252035301011807</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -1570,7 +1570,7 @@
         <v>650</v>
       </c>
       <c r="F3" t="n">
-        <v>8.249122145093745</v>
+        <v>8.265331847337418</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -1597,7 +1597,7 @@
         <v>1016</v>
       </c>
       <c r="F4" t="n">
-        <v>8.320523919408037</v>
+        <v>8.331373152267158</v>
       </c>
       <c r="G4" t="n">
         <v>25</v>
@@ -1624,7 +1624,7 @@
         <v>1381</v>
       </c>
       <c r="F5" t="n">
-        <v>8.304685298771954</v>
+        <v>8.329031300172565</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -1651,7 +1651,7 @@
         <v>285</v>
       </c>
       <c r="F6" t="n">
-        <v>8.258510109442415</v>
+        <v>8.252035301011807</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -1678,7 +1678,7 @@
         <v>650</v>
       </c>
       <c r="F7" t="n">
-        <v>8.249122145093745</v>
+        <v>8.265331847337418</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -1705,7 +1705,7 @@
         <v>1016</v>
       </c>
       <c r="F8" t="n">
-        <v>8.320523919408037</v>
+        <v>8.331373152267158</v>
       </c>
       <c r="G8" t="n">
         <v>25</v>
@@ -1732,7 +1732,7 @@
         <v>1381</v>
       </c>
       <c r="F9" t="n">
-        <v>8.304685298771954</v>
+        <v>8.329031300172565</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -1759,7 +1759,7 @@
         <v>285</v>
       </c>
       <c r="F10" t="n">
-        <v>8.258510109442415</v>
+        <v>8.252035301011807</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -1786,7 +1786,7 @@
         <v>650</v>
       </c>
       <c r="F11" t="n">
-        <v>8.249122145093745</v>
+        <v>8.265331847337418</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -1813,7 +1813,7 @@
         <v>1016</v>
       </c>
       <c r="F12" t="n">
-        <v>8.320523919408037</v>
+        <v>8.331373152267158</v>
       </c>
       <c r="G12" t="n">
         <v>25</v>
@@ -1840,7 +1840,7 @@
         <v>1381</v>
       </c>
       <c r="F13" t="n">
-        <v>8.304685298771954</v>
+        <v>8.329031300172565</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -1867,7 +1867,7 @@
         <v>446</v>
       </c>
       <c r="F14" t="n">
-        <v>5.601084606779181</v>
+        <v>5.799594592429121</v>
       </c>
       <c r="G14" t="n">
         <v>625</v>
@@ -1894,7 +1894,7 @@
         <v>811</v>
       </c>
       <c r="F15" t="n">
-        <v>5.714017162372091</v>
+        <v>5.724272415628232</v>
       </c>
       <c r="G15" t="n">
         <v>600</v>
@@ -1921,10 +1921,10 @@
         <v>1177</v>
       </c>
       <c r="F16" t="n">
-        <v>5.206264511033568</v>
+        <v>5.425883008718891</v>
       </c>
       <c r="G16" t="n">
-        <v>600</v>
+        <v>575</v>
       </c>
     </row>
     <row r="17">
@@ -1948,7 +1948,7 @@
         <v>446</v>
       </c>
       <c r="F17" t="n">
-        <v>5.601084606779181</v>
+        <v>5.799594592429121</v>
       </c>
       <c r="G17" t="n">
         <v>625</v>
@@ -1975,7 +1975,7 @@
         <v>811</v>
       </c>
       <c r="F18" t="n">
-        <v>5.714017162372091</v>
+        <v>5.724272415628232</v>
       </c>
       <c r="G18" t="n">
         <v>600</v>
@@ -2002,10 +2002,10 @@
         <v>1177</v>
       </c>
       <c r="F19" t="n">
-        <v>5.206264511033568</v>
+        <v>5.425883008718891</v>
       </c>
       <c r="G19" t="n">
-        <v>600</v>
+        <v>575</v>
       </c>
     </row>
     <row r="20">
@@ -2029,7 +2029,7 @@
         <v>446</v>
       </c>
       <c r="F20" t="n">
-        <v>5.601084606779181</v>
+        <v>5.799594592429121</v>
       </c>
       <c r="G20" t="n">
         <v>625</v>
@@ -2056,7 +2056,7 @@
         <v>811</v>
       </c>
       <c r="F21" t="n">
-        <v>5.714017162372091</v>
+        <v>5.724272415628232</v>
       </c>
       <c r="G21" t="n">
         <v>600</v>
@@ -2083,10 +2083,10 @@
         <v>1177</v>
       </c>
       <c r="F22" t="n">
-        <v>5.206264511033568</v>
+        <v>5.425883008718891</v>
       </c>
       <c r="G22" t="n">
-        <v>600</v>
+        <v>575</v>
       </c>
     </row>
     <row r="23">
@@ -2110,7 +2110,7 @@
         <v>446</v>
       </c>
       <c r="F23" t="n">
-        <v>5.601084606779181</v>
+        <v>5.799594592429121</v>
       </c>
       <c r="G23" t="n">
         <v>625</v>
@@ -2137,7 +2137,7 @@
         <v>811</v>
       </c>
       <c r="F24" t="n">
-        <v>5.714017162372091</v>
+        <v>5.724272415628232</v>
       </c>
       <c r="G24" t="n">
         <v>600</v>
@@ -2164,10 +2164,10 @@
         <v>1177</v>
       </c>
       <c r="F25" t="n">
-        <v>5.206264511033568</v>
+        <v>5.425883008718891</v>
       </c>
       <c r="G25" t="n">
-        <v>600</v>
+        <v>575</v>
       </c>
     </row>
     <row r="26">
@@ -2191,10 +2191,10 @@
         <v>416</v>
       </c>
       <c r="F26" t="n">
-        <v>2.198760725277861</v>
+        <v>2.199050389369717</v>
       </c>
       <c r="G26" t="n">
-        <v>324.6295659004462</v>
+        <v>324.6294128218001</v>
       </c>
     </row>
     <row r="27">
@@ -2218,7 +2218,7 @@
         <v>781</v>
       </c>
       <c r="F27" t="n">
-        <v>3.619064314380449</v>
+        <v>3.619606235631393</v>
       </c>
       <c r="G27" t="n">
         <v>350</v>
@@ -2245,7 +2245,7 @@
         <v>1147</v>
       </c>
       <c r="F28" t="n">
-        <v>1.494408557860785</v>
+        <v>1.494692662904003</v>
       </c>
       <c r="G28" t="n">
         <v>275</v>
@@ -2272,10 +2272,10 @@
         <v>416</v>
       </c>
       <c r="F29" t="n">
-        <v>2.198760725277861</v>
+        <v>2.199050389369717</v>
       </c>
       <c r="G29" t="n">
-        <v>324.6295659004462</v>
+        <v>324.6294128218001</v>
       </c>
     </row>
     <row r="30">
@@ -2299,7 +2299,7 @@
         <v>781</v>
       </c>
       <c r="F30" t="n">
-        <v>3.619064314380449</v>
+        <v>3.619606235631393</v>
       </c>
       <c r="G30" t="n">
         <v>350</v>
@@ -2326,7 +2326,7 @@
         <v>1147</v>
       </c>
       <c r="F31" t="n">
-        <v>1.494408557860785</v>
+        <v>1.494692662904003</v>
       </c>
       <c r="G31" t="n">
         <v>275</v>
@@ -2353,7 +2353,7 @@
         <v>429</v>
       </c>
       <c r="F32" t="n">
-        <v>1.756136236278242</v>
+        <v>1.75629891650748</v>
       </c>
       <c r="G32" t="n">
         <v>325</v>
@@ -2380,7 +2380,7 @@
         <v>794</v>
       </c>
       <c r="F33" t="n">
-        <v>1.404637434746309</v>
+        <v>1.404878119678743</v>
       </c>
       <c r="G33" t="n">
         <v>275</v>
@@ -2407,7 +2407,7 @@
         <v>1160</v>
       </c>
       <c r="F34" t="n">
-        <v>1.774607934116236</v>
+        <v>1.775297960730243</v>
       </c>
       <c r="G34" t="n">
         <v>300</v>
@@ -2434,7 +2434,7 @@
         <v>429</v>
       </c>
       <c r="F35" t="n">
-        <v>1.756136236278242</v>
+        <v>1.75629891650748</v>
       </c>
       <c r="G35" t="n">
         <v>325</v>
@@ -2461,7 +2461,7 @@
         <v>794</v>
       </c>
       <c r="F36" t="n">
-        <v>1.404637434746309</v>
+        <v>1.404878119678743</v>
       </c>
       <c r="G36" t="n">
         <v>275</v>
@@ -2488,7 +2488,7 @@
         <v>1160</v>
       </c>
       <c r="F37" t="n">
-        <v>1.774607934116236</v>
+        <v>1.775297960730243</v>
       </c>
       <c r="G37" t="n">
         <v>300</v>
@@ -2515,7 +2515,7 @@
         <v>392</v>
       </c>
       <c r="F38" t="n">
-        <v>6.218642363086797</v>
+        <v>6.219102643765745</v>
       </c>
       <c r="G38" t="n">
         <v>375</v>
@@ -2542,7 +2542,7 @@
         <v>757</v>
       </c>
       <c r="F39" t="n">
-        <v>2.667275486404149</v>
+        <v>2.667879848391237</v>
       </c>
       <c r="G39" t="n">
         <v>275</v>
@@ -2569,7 +2569,7 @@
         <v>1123</v>
       </c>
       <c r="F40" t="n">
-        <v>1.91016486282304</v>
+        <v>1.910364104782561</v>
       </c>
       <c r="G40" t="n">
         <v>275</v>
@@ -2596,7 +2596,7 @@
         <v>392</v>
       </c>
       <c r="F41" t="n">
-        <v>6.218642363086797</v>
+        <v>6.219102643765745</v>
       </c>
       <c r="G41" t="n">
         <v>375</v>
@@ -2623,7 +2623,7 @@
         <v>757</v>
       </c>
       <c r="F42" t="n">
-        <v>2.667275486404149</v>
+        <v>2.667879848391237</v>
       </c>
       <c r="G42" t="n">
         <v>275</v>
@@ -2650,7 +2650,7 @@
         <v>1123</v>
       </c>
       <c r="F43" t="n">
-        <v>1.91016486282304</v>
+        <v>1.910364104782561</v>
       </c>
       <c r="G43" t="n">
         <v>275</v>
@@ -2680,7 +2680,7 @@
         <v>10.98946021684051</v>
       </c>
       <c r="G44" t="n">
-        <v>1169.996582964024</v>
+        <v>1166.947191939173</v>
       </c>
     </row>
     <row r="45">
@@ -2707,7 +2707,7 @@
         <v>11.02909468512641</v>
       </c>
       <c r="G45" t="n">
-        <v>1201.80155453776</v>
+        <v>1200.390170187957</v>
       </c>
     </row>
     <row r="46">
@@ -2734,7 +2734,7 @@
         <v>11.07541676774006</v>
       </c>
       <c r="G46" t="n">
-        <v>1162.787457982894</v>
+        <v>1150.102147786943</v>
       </c>
     </row>
     <row r="47">
@@ -2761,7 +2761,7 @@
         <v>6.989670147640976</v>
       </c>
       <c r="G47" t="n">
-        <v>722.8891616148685</v>
+        <v>722.8977391671099</v>
       </c>
     </row>
     <row r="48">
@@ -2785,10 +2785,10 @@
         <v>496</v>
       </c>
       <c r="F48" t="n">
-        <v>7.015346889556285</v>
+        <v>7.015346729218368</v>
       </c>
       <c r="G48" t="n">
-        <v>689.1467950874841</v>
+        <v>689.147681439479</v>
       </c>
     </row>
     <row r="49">
@@ -2812,10 +2812,10 @@
         <v>861</v>
       </c>
       <c r="F49" t="n">
-        <v>7.04366061705954</v>
+        <v>7.043660632884428</v>
       </c>
       <c r="G49" t="n">
-        <v>687.9549343529037</v>
+        <v>687.9765759548468</v>
       </c>
     </row>
     <row r="50">
@@ -2842,7 +2842,7 @@
         <v>7.082644536901525</v>
       </c>
       <c r="G50" t="n">
-        <v>674.8918159371151</v>
+        <v>674.9028563351791</v>
       </c>
     </row>
     <row r="51">
@@ -2869,7 +2869,7 @@
         <v>6.989670147640976</v>
       </c>
       <c r="G51" t="n">
-        <v>696.9330851352745</v>
+        <v>696.9296587599061</v>
       </c>
     </row>
     <row r="52">
@@ -2893,10 +2893,10 @@
         <v>502</v>
       </c>
       <c r="F52" t="n">
-        <v>7.015211162951598</v>
+        <v>7.015211013062076</v>
       </c>
       <c r="G52" t="n">
-        <v>698.2336028814002</v>
+        <v>698.2311625269382</v>
       </c>
     </row>
     <row r="53">
@@ -2920,10 +2920,10 @@
         <v>867</v>
       </c>
       <c r="F53" t="n">
-        <v>7.047831916368094</v>
+        <v>7.047831954663301</v>
       </c>
       <c r="G53" t="n">
-        <v>665.1754650251687</v>
+        <v>665.171884249018</v>
       </c>
     </row>
     <row r="54">
@@ -2947,10 +2947,10 @@
         <v>1233</v>
       </c>
       <c r="F54" t="n">
-        <v>7.08299744589133</v>
+        <v>7.08299744934908</v>
       </c>
       <c r="G54" t="n">
-        <v>674.0995413255899</v>
+        <v>674.0966184177332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>